<commit_message>
Implementação final. Projeto para fazer medições entre o banco de dados MySQL (Relacional) e o banco de dados MongoDB (NoSQL)
</commit_message>
<xml_diff>
--- a/Terra/Resultado pesquisa.xlsx
+++ b/Terra/Resultado pesquisa.xlsx
@@ -4,53 +4,172 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="26520" windowHeight="11660"/>
+    <workbookView windowWidth="26520" windowHeight="11660" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Tabela" sheetId="1" r:id="rId1"/>
+    <sheet name="Servidor" sheetId="2" r:id="rId2"/>
+    <sheet name="Resultados singular" sheetId="3" r:id="rId3"/>
+    <sheet name="Resultados massa" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8">
-  <si>
-    <t>Comando</t>
-  </si>
-  <si>
-    <t>Tipo comando</t>
-  </si>
-  <si>
-    <t>Banco</t>
-  </si>
-  <si>
-    <t>Duração</t>
-  </si>
-  <si>
-    <t>INSERT into...</t>
-  </si>
-  <si>
-    <t>Quantidade comandos INSERT</t>
-  </si>
-  <si>
-    <t>Média de tempo do banco de dados</t>
-  </si>
-  <si>
-    <t>Com thread</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47">
+  <si>
+    <t>Ação</t>
+  </si>
+  <si>
+    <t>Requisições de comando</t>
+  </si>
+  <si>
+    <t>Threads</t>
+  </si>
+  <si>
+    <t>Inserção</t>
+  </si>
+  <si>
+    <t>Consulta</t>
+  </si>
+  <si>
+    <t>Procesador</t>
+  </si>
+  <si>
+    <t>Memória</t>
+  </si>
+  <si>
+    <t>Sistema Operacional</t>
+  </si>
+  <si>
+    <t>2048M</t>
+  </si>
+  <si>
+    <t>Debian 7</t>
+  </si>
+  <si>
+    <t>Média de Inserção para 1 Thread</t>
+  </si>
+  <si>
+    <t>Quantidade</t>
+  </si>
+  <si>
+    <t>MySQL</t>
+  </si>
+  <si>
+    <t>MongoDB</t>
+  </si>
+  <si>
+    <t>6 ms</t>
+  </si>
+  <si>
+    <t>7 ms</t>
+  </si>
+  <si>
+    <t>3 ms</t>
+  </si>
+  <si>
+    <t>5 ms</t>
+  </si>
+  <si>
+    <t>4 ms</t>
+  </si>
+  <si>
+    <t>Média de Inserção para 10 Thread</t>
+  </si>
+  <si>
+    <t>14 ms</t>
+  </si>
+  <si>
+    <t>27 ms</t>
+  </si>
+  <si>
+    <t>12 ms</t>
+  </si>
+  <si>
+    <t>17 ms</t>
+  </si>
+  <si>
+    <t>11 ms</t>
+  </si>
+  <si>
+    <t>54 ms</t>
+  </si>
+  <si>
+    <t>Média de Inserção para 100 Thread</t>
+  </si>
+  <si>
+    <t>36 ms</t>
+  </si>
+  <si>
+    <t>103 ms</t>
+  </si>
+  <si>
+    <t>149 ms</t>
+  </si>
+  <si>
+    <t>Tempo de Inserção</t>
+  </si>
+  <si>
+    <t>Média por Consulta</t>
+  </si>
+  <si>
+    <t>675 ms (0s)</t>
+  </si>
+  <si>
+    <t>457 ms (0s)</t>
+  </si>
+  <si>
+    <t>670.000 ns (0s)</t>
+  </si>
+  <si>
+    <t>90.000 ns (0s)</t>
+  </si>
+  <si>
+    <t>3 s</t>
+  </si>
+  <si>
+    <t>1 s</t>
+  </si>
+  <si>
+    <t>618.000 ns (0s)</t>
+  </si>
+  <si>
+    <t>17.000 ns (0s)</t>
+  </si>
+  <si>
+    <t>25 s</t>
+  </si>
+  <si>
+    <t>1 ms (0s)</t>
+  </si>
+  <si>
+    <t>3.000 ns (0s)</t>
+  </si>
+  <si>
+    <t>238 s (3m)</t>
+  </si>
+  <si>
+    <t>22 s</t>
+  </si>
+  <si>
+    <t>5 ms (0s)</t>
+  </si>
+  <si>
+    <t>477 ns (0s)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="#,##0_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -83,7 +202,7 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -96,9 +215,21 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -413,11 +544,11 @@
         </a:custGeom>
         <a:gradFill rotWithShape="0">
           <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="BBD5F0"/>
+            </a:gs>
             <a:gs pos="100000">
               <a:srgbClr val="9CBEE0"/>
-            </a:gs>
-            <a:gs pos="0">
-              <a:srgbClr val="BBD5F0"/>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
@@ -441,47 +572,66 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="14" outlineLevelRow="4" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="14" outlineLevelRow="4" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="26.6" customWidth="1"/>
-    <col min="2" max="2" width="23.2" customWidth="1"/>
-    <col min="3" max="3" width="10.7" customWidth="1"/>
+    <col min="1" max="1" width="7.67" customWidth="1"/>
+    <col min="2" max="2" width="16.265" style="4" customWidth="1"/>
+    <col min="3" max="3" width="8.4" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
+      <c r="B2" s="4">
+        <v>100</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
+      <c r="B3" s="4">
+        <v>1000</v>
+      </c>
+      <c r="C3" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3">
+      <c r="B4" s="4">
+        <v>10000</v>
+      </c>
+      <c r="C4" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3">
+      <c r="B5" s="4">
+        <v>90000</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1000</v>
       </c>
     </row>
   </sheetData>
@@ -493,14 +643,41 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="14"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="8.8" style="4"/>
+    <col min="3" max="3" width="18.3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>
@@ -509,14 +686,316 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="14"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="14" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="10.1" style="3" customWidth="1"/>
+    <col min="3" max="3" width="8.8" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="3">
+        <v>100</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="3">
+        <v>1000</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="3">
+        <v>10000</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="3">
+        <v>90000</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="3">
+        <v>1000</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="3">
+        <v>10000</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="3">
+        <v>100000</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="3">
+        <v>10000</v>
+      </c>
+      <c r="B19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="3">
+        <v>100000</v>
+      </c>
+      <c r="B20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A17:C17"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="14" outlineLevelRow="5" outlineLevelCol="6"/>
+  <cols>
+    <col min="2" max="2" width="9.43" customWidth="1"/>
+    <col min="3" max="3" width="10.6" customWidth="1"/>
+    <col min="6" max="6" width="13.1" customWidth="1"/>
+    <col min="7" max="7" width="12.1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="E1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="3">
+        <v>100</v>
+      </c>
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="3">
+        <v>100</v>
+      </c>
+      <c r="F3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="3">
+        <v>1000</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1000</v>
+      </c>
+      <c r="F4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="3">
+        <v>10000</v>
+      </c>
+      <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="3">
+        <v>10000</v>
+      </c>
+      <c r="F5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="3">
+        <v>90000</v>
+      </c>
+      <c r="B6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="3">
+        <v>90000</v>
+      </c>
+      <c r="F6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="E1:G1"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>

</xml_diff>